<commit_message>
updated BOM and Revised To do list
</commit_message>
<xml_diff>
--- a/Structural_BOM_Rover.xlsx
+++ b/Structural_BOM_Rover.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kulde\OneDrive\Desktop\Romeo_007\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1F5DDE-B047-4899-AFB7-087166432963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9655F54-9BCF-4852-AC2F-F2E2DF577CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8B20D429-B29D-4754-92B2-C46CE5D0CC7C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Component</t>
   </si>
@@ -128,15 +128,9 @@
     <t>15mm dia hollow aluminium rod</t>
   </si>
   <si>
-    <t>Sliding Nuts 20*20 + Bolts</t>
-  </si>
-  <si>
     <t>Siliding Nuts 40*40 (M8) + Bolts</t>
   </si>
   <si>
-    <t>M8 bolts length 80mm</t>
-  </si>
-  <si>
     <t>https://robu.in/product/easymech-aluminum-extrusion-end-cap-for-20x20-4-pcs/</t>
   </si>
   <si>
@@ -156,6 +150,30 @@
   </si>
   <si>
     <t>Jaw Turn Buckle (Pivot joint)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/TRENDYNEST-Stainless-Closed-Turnbuckle-Rigging/dp/B0FKMX5RNV</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/uxcell-Screws-Washers-Stainless-Hexagon/dp/B098D9565X?th=1</t>
+  </si>
+  <si>
+    <t>M8 bolts length 65mm</t>
+  </si>
+  <si>
+    <t>M8 nylon lock nuts</t>
+  </si>
+  <si>
+    <t>https://www.amazon.in/Stainless-Steel-Nylon-Lock-Thread/dp/B0FHGFLB6Y</t>
+  </si>
+  <si>
+    <t>https://robu.in/product/easymech-sliding-m5-t-nut-for-20x20-aluminium-profile-10-pcs/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sliding Nuts 20*20 </t>
+  </si>
+  <si>
+    <t>https://robokits.co.in/mechanical-parts/aluminium-profile-accessories/slider-square-fitting-m8-nut-for-4040-aluminium-profile-moq-10pcs?products_id=3996:43e04dd08bb1305428b0c9c8d8a2660a</t>
   </si>
 </sst>
 </file>
@@ -578,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63C0E43-6284-4239-8CC0-FD6AC2EB404A}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,7 +785,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -776,12 +794,14 @@
         <v>1.5</v>
       </c>
       <c r="E9" s="1">
-        <f>B9*D9</f>
+        <f t="shared" ref="E9:E14" si="0">B9*D9</f>
         <v>6</v>
       </c>
       <c r="F9"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -794,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="1">
-        <f>B10*D10</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F10"/>
@@ -805,7 +825,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>40</v>
@@ -814,28 +834,32 @@
         <v>2</v>
       </c>
       <c r="E11" s="1">
-        <f>B11*D11</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="F11"/>
       <c r="G11" s="1"/>
+      <c r="H11" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" s="1">
-        <f>B12*D12</f>
-        <v>80</v>
+        <f t="shared" si="0"/>
+        <v>160</v>
       </c>
       <c r="F12"/>
       <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -848,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="1">
-        <f>B13*D13</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F13"/>
@@ -868,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="1">
-        <f>B14*D14</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F14"/>
@@ -907,18 +931,18 @@
         <v>1.5</v>
       </c>
       <c r="E16" s="1">
-        <f>B16*D16</f>
+        <f t="shared" ref="E16:E22" si="1">B16*D16</f>
         <v>37.5</v>
       </c>
       <c r="F16"/>
       <c r="G16" s="1"/>
       <c r="H16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>8</v>
@@ -927,18 +951,18 @@
         <v>2</v>
       </c>
       <c r="E17" s="1">
-        <f>B17*D17</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F17"/>
       <c r="G17" s="1"/>
       <c r="H17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -947,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="1">
-        <f>B18*D18</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="F18"/>
@@ -958,7 +982,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19">
         <v>40</v>
@@ -967,44 +991,54 @@
         <v>1.5</v>
       </c>
       <c r="E19" s="1">
-        <f>B19*D19</f>
+        <f t="shared" si="1"/>
         <v>60</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="D20" s="1">
-        <v>1.5</v>
-      </c>
       <c r="E20" s="1">
-        <f>B20*D20</f>
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21">
+        <v>41</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22">
         <v>1</v>
       </c>
-      <c r="D21" s="1">
-        <v>2</v>
-      </c>
-      <c r="E21" s="1">
-        <f>B21*D21</f>
-        <v>2</v>
-      </c>
-      <c r="G21">
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G22">
         <v>175</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>38</v>
+      <c r="H22" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1020,7 +1054,12 @@
     <hyperlink ref="H17" r:id="rId8" xr:uid="{5B61EAC7-FAA9-4738-ADFE-4832EEF3165D}"/>
     <hyperlink ref="H18" r:id="rId9" xr:uid="{BA503AA3-3878-4C77-8CE5-6D535A7CF764}"/>
     <hyperlink ref="H16" r:id="rId10" xr:uid="{B1DF8262-3868-4D2E-BADC-B5A8A2E46E32}"/>
-    <hyperlink ref="H21" r:id="rId11" xr:uid="{D27A027F-3EFF-4D0A-B918-2D8880A48F24}"/>
+    <hyperlink ref="H22" r:id="rId11" xr:uid="{D27A027F-3EFF-4D0A-B918-2D8880A48F24}"/>
+    <hyperlink ref="H9" r:id="rId12" xr:uid="{1EDA434E-70C6-421D-A333-2774E8B1CE04}"/>
+    <hyperlink ref="H20" r:id="rId13" xr:uid="{B49CB4B7-F871-470C-94F0-27BB38BF181A}"/>
+    <hyperlink ref="H21" r:id="rId14" xr:uid="{E8A1F4A3-AC97-4B6C-B8DF-58AA04D2303D}"/>
+    <hyperlink ref="H11" r:id="rId15" xr:uid="{4AE8AD4C-EC66-40BB-8F69-697F7C0865F5}"/>
+    <hyperlink ref="H19" r:id="rId16" xr:uid="{0B767714-0273-49A5-B1EA-55BCFFCB10B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>